<commit_message>
Update Mark Williamson OTJ Tracker.xlsx
</commit_message>
<xml_diff>
--- a/Mark Williamson OTJ Tracker.xlsx
+++ b/Mark Williamson OTJ Tracker.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="337" uniqueCount="270">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="338" uniqueCount="271">
   <si>
     <t xml:space="preserve">Apprenticeship Training Log </t>
   </si>
@@ -182,6 +182,9 @@
   </si>
   <si>
     <t xml:space="preserve">S6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Created python code to access an API and pull data into a cloud-based database and then used a scheduled linux cron job to trigger data ingestion</t>
   </si>
   <si>
     <t xml:space="preserve">GRAND TOTAL</t>
@@ -2321,9 +2324,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>17</xdr:col>
-      <xdr:colOff>293040</xdr:colOff>
+      <xdr:colOff>292680</xdr:colOff>
       <xdr:row>5</xdr:row>
-      <xdr:rowOff>156240</xdr:rowOff>
+      <xdr:rowOff>155880</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2337,7 +2340,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="12153240" y="181080"/>
-          <a:ext cx="1268280" cy="1262160"/>
+          <a:ext cx="1267920" cy="1261800"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2359,9 +2362,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>17</xdr:col>
-      <xdr:colOff>53640</xdr:colOff>
+      <xdr:colOff>53280</xdr:colOff>
       <xdr:row>32</xdr:row>
-      <xdr:rowOff>129960</xdr:rowOff>
+      <xdr:rowOff>129600</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2375,7 +2378,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="1030680" y="4953240"/>
-          <a:ext cx="12151440" cy="1607400"/>
+          <a:ext cx="12151080" cy="1607040"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2570,8 +2573,8 @@
   </sheetPr>
   <dimension ref="A1:AP312"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A34" colorId="64" zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B50" activeCellId="0" sqref="B50"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A49" colorId="64" zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B72" activeCellId="0" sqref="B72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4574,14 +4577,20 @@
       <c r="AO39" s="2"/>
       <c r="AP39" s="2"/>
     </row>
-    <row r="40" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="40" customFormat="false" ht="38.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A40" s="14"/>
-      <c r="B40" s="30"/>
+      <c r="B40" s="30" t="s">
+        <v>50</v>
+      </c>
       <c r="C40" s="57"/>
-      <c r="D40" s="66"/>
+      <c r="D40" s="58" t="n">
+        <v>45918</v>
+      </c>
       <c r="E40" s="19"/>
       <c r="F40" s="19"/>
-      <c r="G40" s="67"/>
+      <c r="G40" s="59" t="n">
+        <v>8</v>
+      </c>
       <c r="H40" s="54"/>
       <c r="I40" s="2"/>
       <c r="J40" s="2"/>
@@ -5508,7 +5517,7 @@
       <c r="F61" s="73"/>
       <c r="G61" s="36" t="n">
         <f aca="false">SUM(G36:G60)</f>
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="H61" s="54"/>
       <c r="I61" s="2"/>
@@ -5593,7 +5602,7 @@
     <row r="63" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="14"/>
       <c r="B63" s="77" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C63" s="77"/>
       <c r="D63" s="78"/>
@@ -5601,7 +5610,7 @@
       <c r="F63" s="79"/>
       <c r="G63" s="80" t="n">
         <f aca="false">G61+G19+G28+G62</f>
-        <v>265</v>
+        <v>273</v>
       </c>
       <c r="H63" s="81"/>
       <c r="I63" s="2"/>
@@ -5728,11 +5737,10 @@
     <row r="66" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="14"/>
       <c r="B66" s="27" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C66" s="27" t="n">
-        <f aca="false">'List - Hide'!AC11</f>
-        <v>487</v>
+        <v>359</v>
       </c>
       <c r="D66" s="2"/>
       <c r="F66" s="2"/>
@@ -5776,11 +5784,11 @@
     <row r="67" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="14"/>
       <c r="B67" s="27" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C67" s="27" t="n">
         <f aca="false">G63</f>
-        <v>265</v>
+        <v>273</v>
       </c>
       <c r="D67" s="2"/>
       <c r="F67" s="2"/>
@@ -5824,11 +5832,11 @@
     <row r="68" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="14"/>
       <c r="B68" s="27" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C68" s="40" t="n">
         <f aca="false">C66-C67</f>
-        <v>222</v>
+        <v>86</v>
       </c>
       <c r="D68" s="2"/>
       <c r="F68" s="2"/>
@@ -11823,78 +11831,78 @@
   <sheetData>
     <row r="2" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B2" s="82" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="83" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C4" s="84" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B5" s="85" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C5" s="85"/>
     </row>
     <row r="6" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B6" s="85" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C6" s="85"/>
     </row>
     <row r="7" customFormat="false" ht="29.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B7" s="85" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C7" s="85"/>
     </row>
     <row r="8" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B8" s="85" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C8" s="85" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="51.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B9" s="85" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C9" s="86" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B10" s="85" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C10" s="85" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="30.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B11" s="85" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="C11" s="85" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="27.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B12" s="85" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C12" s="85" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="33" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B13" s="85" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="C13" s="85" t="s">
         <v>10</v>
@@ -11902,15 +11910,15 @@
     </row>
     <row r="14" customFormat="false" ht="30.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B14" s="85" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C14" s="85" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B15" s="85" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C15" s="85"/>
     </row>
@@ -12021,24 +12029,24 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="88" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B1" s="49" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C1" s="49" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="89" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B2" s="90" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C2" s="91" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="D2" s="68"/>
       <c r="E2" s="68"/>
@@ -12093,13 +12101,13 @@
     </row>
     <row r="3" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="89" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B3" s="91" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="C3" s="91" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="D3" s="68"/>
       <c r="E3" s="68"/>
@@ -12154,13 +12162,13 @@
     </row>
     <row r="4" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="89" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="B4" s="91" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C4" s="91" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="D4" s="68"/>
       <c r="E4" s="68"/>
@@ -12215,13 +12223,13 @@
     </row>
     <row r="5" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="89" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="B5" s="91" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C5" s="91" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D5" s="68"/>
       <c r="E5" s="68"/>
@@ -12276,13 +12284,13 @@
     </row>
     <row r="6" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="89" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="B6" s="91" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="C6" s="91" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="D6" s="68"/>
       <c r="E6" s="68"/>
@@ -12337,13 +12345,13 @@
     </row>
     <row r="7" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="89" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="B7" s="91" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="C7" s="91" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="D7" s="68"/>
       <c r="E7" s="68"/>
@@ -12398,10 +12406,10 @@
     </row>
     <row r="8" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="89" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="B8" s="91" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="C8" s="68"/>
       <c r="D8" s="68"/>
@@ -12457,10 +12465,10 @@
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="89" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="B9" s="91" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="C9" s="68"/>
       <c r="D9" s="68"/>
@@ -12516,10 +12524,10 @@
     </row>
     <row r="10" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="89" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="B10" s="91" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="C10" s="68"/>
       <c r="D10" s="68"/>
@@ -12575,10 +12583,10 @@
     </row>
     <row r="11" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="89" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="B11" s="91" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="C11" s="68"/>
       <c r="D11" s="68"/>
@@ -12634,10 +12642,10 @@
     </row>
     <row r="12" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="89" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="B12" s="68" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="C12" s="68"/>
       <c r="D12" s="68"/>
@@ -12693,10 +12701,10 @@
     </row>
     <row r="13" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="89" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="B13" s="68" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="C13" s="68"/>
       <c r="D13" s="68"/>
@@ -12752,10 +12760,10 @@
     </row>
     <row r="14" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="89" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="B14" s="68" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="C14" s="68"/>
       <c r="D14" s="68"/>
@@ -12811,10 +12819,10 @@
     </row>
     <row r="15" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="89" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="B15" s="68" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="C15" s="68"/>
       <c r="D15" s="68"/>
@@ -12870,10 +12878,10 @@
     </row>
     <row r="16" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="89" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="B16" s="68" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="C16" s="68"/>
       <c r="D16" s="68"/>
@@ -12929,10 +12937,10 @@
     </row>
     <row r="17" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="89" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="B17" s="68" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="C17" s="68"/>
       <c r="D17" s="68"/>
@@ -12988,10 +12996,10 @@
     </row>
     <row r="18" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="89" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="B18" s="68" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="C18" s="68"/>
       <c r="D18" s="68"/>
@@ -13047,10 +13055,10 @@
     </row>
     <row r="19" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="89" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="B19" s="68" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="C19" s="68"/>
       <c r="D19" s="68"/>
@@ -13106,10 +13114,10 @@
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="89" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="B20" s="68" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="C20" s="68"/>
       <c r="D20" s="68"/>
@@ -13165,10 +13173,10 @@
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="89" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="B21" s="68" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="C21" s="68"/>
       <c r="D21" s="68"/>
@@ -13224,10 +13232,10 @@
     </row>
     <row r="22" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="89" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="B22" s="68" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="C22" s="68"/>
       <c r="D22" s="68"/>
@@ -13283,10 +13291,10 @@
     </row>
     <row r="23" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="89" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="B23" s="68" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="C23" s="68"/>
       <c r="D23" s="68"/>
@@ -13342,10 +13350,10 @@
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="89" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="B24" s="68" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="C24" s="68"/>
       <c r="D24" s="68"/>
@@ -13401,10 +13409,10 @@
     </row>
     <row r="25" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="89" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="B25" s="68" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="C25" s="68"/>
       <c r="D25" s="68"/>
@@ -13460,10 +13468,10 @@
     </row>
     <row r="26" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="89" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="B26" s="68" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="C26" s="68"/>
       <c r="D26" s="68"/>
@@ -13519,10 +13527,10 @@
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="89" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="B27" s="68" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="C27" s="68"/>
       <c r="D27" s="68"/>
@@ -13578,10 +13586,10 @@
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="89" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="B28" s="68" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="C28" s="68"/>
       <c r="D28" s="68"/>
@@ -13637,10 +13645,10 @@
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="89" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="B29" s="68" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="C29" s="68"/>
       <c r="D29" s="68"/>
@@ -13696,10 +13704,10 @@
     </row>
     <row r="30" s="89" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="89" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="B30" s="91" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="C30" s="91"/>
       <c r="D30" s="91"/>
@@ -13755,7 +13763,7 @@
     </row>
     <row r="31" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="89" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="B31" s="68"/>
       <c r="C31" s="68"/>
@@ -25426,10 +25434,10 @@
       <c r="B1" s="92"/>
       <c r="C1" s="92"/>
       <c r="D1" s="93" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="E1" s="94" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="F1" s="94" t="s">
         <v>11</v>
@@ -25468,28 +25476,28 @@
         <v>22</v>
       </c>
       <c r="R1" s="94" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="S1" s="94" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="T1" s="94" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="U1" s="94" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="V1" s="94" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="W1" s="94" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="X1" s="94" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="Y1" s="95" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="Z1" s="92"/>
       <c r="AA1" s="92"/>
@@ -25503,13 +25511,13 @@
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="96" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="B2" s="97" t="n">
         <v>1</v>
       </c>
       <c r="C2" s="98" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="D2" s="99"/>
       <c r="E2" s="100" t="n">
@@ -25564,7 +25572,7 @@
       <c r="A3" s="96"/>
       <c r="B3" s="97"/>
       <c r="C3" s="103" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="D3" s="104"/>
       <c r="E3" s="102"/>
@@ -25616,7 +25624,7 @@
       <c r="A4" s="96"/>
       <c r="B4" s="97"/>
       <c r="C4" s="103" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="D4" s="104"/>
       <c r="E4" s="102"/>
@@ -25668,7 +25676,7 @@
       <c r="A5" s="96"/>
       <c r="B5" s="97"/>
       <c r="C5" s="103" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="D5" s="104"/>
       <c r="E5" s="102"/>
@@ -25722,7 +25730,7 @@
         <v>2</v>
       </c>
       <c r="C6" s="103" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="D6" s="104"/>
       <c r="E6" s="102"/>
@@ -25776,7 +25784,7 @@
       <c r="A7" s="96"/>
       <c r="B7" s="106"/>
       <c r="C7" s="103" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="D7" s="104"/>
       <c r="E7" s="102"/>
@@ -25828,7 +25836,7 @@
       <c r="A8" s="96"/>
       <c r="B8" s="106"/>
       <c r="C8" s="103" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="D8" s="104"/>
       <c r="E8" s="102"/>
@@ -25879,7 +25887,7 @@
       <c r="A9" s="96"/>
       <c r="B9" s="106"/>
       <c r="C9" s="103" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="D9" s="104"/>
       <c r="E9" s="102"/>
@@ -25919,7 +25927,7 @@
       <c r="Z9" s="102"/>
       <c r="AA9" s="102"/>
       <c r="AB9" s="102" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="AC9" s="102" t="n">
         <f aca="false">E2</f>
@@ -25937,7 +25945,7 @@
         <v>3</v>
       </c>
       <c r="C10" s="103" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="D10" s="104"/>
       <c r="E10" s="102"/>
@@ -25979,13 +25987,13 @@
       <c r="Z10" s="102"/>
       <c r="AA10" s="102"/>
       <c r="AB10" s="107" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="AC10" s="102"/>
       <c r="AD10" s="102"/>
       <c r="AE10" s="102"/>
       <c r="AF10" s="102" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="AG10" s="102"/>
       <c r="AH10" s="102"/>
@@ -25994,7 +26002,7 @@
       <c r="A11" s="96"/>
       <c r="B11" s="106"/>
       <c r="C11" s="103" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="D11" s="104"/>
       <c r="E11" s="102"/>
@@ -26034,7 +26042,7 @@
       <c r="Z11" s="102"/>
       <c r="AA11" s="102"/>
       <c r="AB11" s="108" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="AC11" s="109" t="n">
         <f aca="false">Y79+AC9</f>
@@ -26050,7 +26058,7 @@
       <c r="A12" s="96"/>
       <c r="B12" s="106"/>
       <c r="C12" s="103" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="D12" s="104"/>
       <c r="E12" s="102"/>
@@ -26091,16 +26099,16 @@
       <c r="AA12" s="102"/>
       <c r="AB12" s="102"/>
       <c r="AC12" s="110" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="AD12" s="110" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="AE12" s="111" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="AF12" s="111" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="AG12" s="102"/>
       <c r="AH12" s="102"/>
@@ -26109,7 +26117,7 @@
       <c r="A13" s="96"/>
       <c r="B13" s="106"/>
       <c r="C13" s="103" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="D13" s="104"/>
       <c r="E13" s="102"/>
@@ -26129,7 +26137,7 @@
       <c r="Q13" s="105"/>
       <c r="R13" s="102"/>
       <c r="S13" s="112" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="T13" s="102"/>
       <c r="U13" s="104" t="n">
@@ -26178,7 +26186,7 @@
         <v>4</v>
       </c>
       <c r="C14" s="103" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="D14" s="104"/>
       <c r="E14" s="102"/>
@@ -26244,7 +26252,7 @@
       <c r="A15" s="96"/>
       <c r="B15" s="106"/>
       <c r="C15" s="103" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="D15" s="104"/>
       <c r="E15" s="102"/>
@@ -26308,7 +26316,7 @@
       <c r="A16" s="96"/>
       <c r="B16" s="106"/>
       <c r="C16" s="103" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="D16" s="104"/>
       <c r="E16" s="102"/>
@@ -26372,7 +26380,7 @@
       <c r="A17" s="96"/>
       <c r="B17" s="106"/>
       <c r="C17" s="103" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="D17" s="104"/>
       <c r="E17" s="102"/>
@@ -26438,7 +26446,7 @@
         <v>5</v>
       </c>
       <c r="C18" s="103" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="D18" s="104"/>
       <c r="E18" s="102"/>
@@ -26504,7 +26512,7 @@
       <c r="A19" s="96"/>
       <c r="B19" s="106"/>
       <c r="C19" s="103" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="D19" s="104"/>
       <c r="E19" s="102"/>
@@ -26569,7 +26577,7 @@
       <c r="A20" s="96"/>
       <c r="B20" s="106"/>
       <c r="C20" s="103" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="D20" s="104"/>
       <c r="E20" s="102"/>
@@ -26633,7 +26641,7 @@
       <c r="A21" s="96"/>
       <c r="B21" s="106"/>
       <c r="C21" s="103" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="D21" s="104"/>
       <c r="E21" s="102"/>
@@ -26699,7 +26707,7 @@
         <v>6</v>
       </c>
       <c r="C22" s="103" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="D22" s="104"/>
       <c r="E22" s="102"/>
@@ -26764,7 +26772,7 @@
       <c r="A23" s="96"/>
       <c r="B23" s="106"/>
       <c r="C23" s="103" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="D23" s="104"/>
       <c r="E23" s="102"/>
@@ -26784,7 +26792,7 @@
       <c r="Q23" s="105"/>
       <c r="R23" s="102"/>
       <c r="S23" s="112" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="T23" s="102"/>
       <c r="U23" s="104" t="n">
@@ -26830,7 +26838,7 @@
       <c r="A24" s="96"/>
       <c r="B24" s="106"/>
       <c r="C24" s="103" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="D24" s="104"/>
       <c r="E24" s="102"/>
@@ -26892,7 +26900,7 @@
       <c r="A25" s="96"/>
       <c r="B25" s="106"/>
       <c r="C25" s="103" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="D25" s="104"/>
       <c r="E25" s="102"/>
@@ -26953,7 +26961,7 @@
         <v>7</v>
       </c>
       <c r="C26" s="103" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="D26" s="104"/>
       <c r="E26" s="102"/>
@@ -26997,13 +27005,13 @@
       <c r="AA26" s="102"/>
       <c r="AB26" s="92"/>
       <c r="AC26" s="110" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="AD26" s="110" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="AE26" s="111" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="AF26" s="102"/>
       <c r="AG26" s="102"/>
@@ -27012,7 +27020,7 @@
       <c r="A27" s="96"/>
       <c r="B27" s="106"/>
       <c r="C27" s="103" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="D27" s="104"/>
       <c r="E27" s="102"/>
@@ -27053,7 +27061,7 @@
       <c r="Z27" s="102"/>
       <c r="AA27" s="102"/>
       <c r="AB27" s="121" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="AC27" s="114" t="n">
         <v>10</v>
@@ -27069,7 +27077,7 @@
       <c r="A28" s="96"/>
       <c r="B28" s="106"/>
       <c r="C28" s="103" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="D28" s="104"/>
       <c r="E28" s="102"/>
@@ -27110,7 +27118,7 @@
       <c r="Z28" s="102"/>
       <c r="AA28" s="102"/>
       <c r="AB28" s="121" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="AC28" s="114" t="n">
         <v>10</v>
@@ -27126,7 +27134,7 @@
       <c r="A29" s="96"/>
       <c r="B29" s="106"/>
       <c r="C29" s="103" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="D29" s="104"/>
       <c r="E29" s="102"/>
@@ -27164,11 +27172,11 @@
         <v>7.5</v>
       </c>
       <c r="Z29" s="102" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="AA29" s="102"/>
       <c r="AB29" s="121" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="AC29" s="114" t="n">
         <v>10</v>
@@ -27186,7 +27194,7 @@
         <v>8</v>
       </c>
       <c r="C30" s="103" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="D30" s="104"/>
       <c r="E30" s="102"/>
@@ -27227,7 +27235,7 @@
       </c>
       <c r="AA30" s="102"/>
       <c r="AB30" s="121" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="AC30" s="114" t="n">
         <v>10</v>
@@ -27243,7 +27251,7 @@
       <c r="A31" s="96"/>
       <c r="B31" s="106"/>
       <c r="C31" s="103" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="D31" s="104"/>
       <c r="E31" s="102"/>
@@ -27283,7 +27291,7 @@
       <c r="Z31" s="102"/>
       <c r="AA31" s="102"/>
       <c r="AB31" s="121" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="AC31" s="117" t="n">
         <v>10</v>
@@ -27299,7 +27307,7 @@
       <c r="A32" s="96"/>
       <c r="B32" s="106"/>
       <c r="C32" s="103" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="D32" s="104"/>
       <c r="E32" s="102"/>
@@ -27350,7 +27358,7 @@
       <c r="A33" s="96"/>
       <c r="B33" s="106"/>
       <c r="C33" s="103" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="D33" s="104"/>
       <c r="E33" s="102"/>
@@ -27370,7 +27378,7 @@
       <c r="Q33" s="105"/>
       <c r="R33" s="102"/>
       <c r="S33" s="112" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="T33" s="102"/>
       <c r="U33" s="104" t="n">
@@ -27399,7 +27407,7 @@
         <v>9</v>
       </c>
       <c r="C34" s="103" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="D34" s="104"/>
       <c r="E34" s="102"/>
@@ -27444,7 +27452,7 @@
       <c r="A35" s="96"/>
       <c r="B35" s="106"/>
       <c r="C35" s="103" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="D35" s="104"/>
       <c r="E35" s="102"/>
@@ -27488,7 +27496,7 @@
       <c r="A36" s="96"/>
       <c r="B36" s="106"/>
       <c r="C36" s="103" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="D36" s="104"/>
       <c r="E36" s="102"/>
@@ -27526,7 +27534,7 @@
         <v>7.5</v>
       </c>
       <c r="Z36" s="102" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="AA36" s="102"/>
     </row>
@@ -27534,7 +27542,7 @@
       <c r="A37" s="96"/>
       <c r="B37" s="106"/>
       <c r="C37" s="103" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="D37" s="104"/>
       <c r="E37" s="102"/>
@@ -27580,7 +27588,7 @@
         <v>10</v>
       </c>
       <c r="C38" s="103" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="D38" s="104"/>
       <c r="E38" s="102"/>
@@ -27627,7 +27635,7 @@
       <c r="A39" s="96"/>
       <c r="B39" s="106"/>
       <c r="C39" s="103" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="D39" s="104"/>
       <c r="E39" s="102"/>
@@ -27673,7 +27681,7 @@
       <c r="A40" s="96"/>
       <c r="B40" s="106"/>
       <c r="C40" s="103" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="D40" s="104"/>
       <c r="E40" s="102"/>
@@ -27718,7 +27726,7 @@
       <c r="A41" s="96"/>
       <c r="B41" s="106"/>
       <c r="C41" s="103" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="D41" s="104"/>
       <c r="E41" s="102"/>
@@ -27771,7 +27779,7 @@
         <v>11</v>
       </c>
       <c r="C42" s="103" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="D42" s="104"/>
       <c r="E42" s="102"/>
@@ -27823,7 +27831,7 @@
       <c r="A43" s="96"/>
       <c r="B43" s="106"/>
       <c r="C43" s="103" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="D43" s="104"/>
       <c r="E43" s="102"/>
@@ -27843,7 +27851,7 @@
       <c r="Q43" s="105"/>
       <c r="R43" s="102"/>
       <c r="S43" s="112" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="T43" s="102"/>
       <c r="U43" s="104" t="n">
@@ -27877,7 +27885,7 @@
       <c r="A44" s="96"/>
       <c r="B44" s="106"/>
       <c r="C44" s="103" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="D44" s="104"/>
       <c r="E44" s="102"/>
@@ -27928,7 +27936,7 @@
       <c r="A45" s="96"/>
       <c r="B45" s="106"/>
       <c r="C45" s="103" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="D45" s="104"/>
       <c r="E45" s="102"/>
@@ -27981,7 +27989,7 @@
         <v>12</v>
       </c>
       <c r="C46" s="103" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="D46" s="104"/>
       <c r="E46" s="102"/>
@@ -28034,7 +28042,7 @@
       <c r="A47" s="96"/>
       <c r="B47" s="106"/>
       <c r="C47" s="103" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="D47" s="104"/>
       <c r="E47" s="102"/>
@@ -28085,7 +28093,7 @@
       <c r="A48" s="96"/>
       <c r="B48" s="106"/>
       <c r="C48" s="103" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="D48" s="104"/>
       <c r="E48" s="102"/>
@@ -28123,7 +28131,7 @@
         <v>9.5</v>
       </c>
       <c r="Z48" s="102" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="AA48" s="102"/>
       <c r="AB48" s="102"/>
@@ -28138,7 +28146,7 @@
       <c r="A49" s="96"/>
       <c r="B49" s="106"/>
       <c r="C49" s="103" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="D49" s="104"/>
       <c r="E49" s="102"/>
@@ -28191,7 +28199,7 @@
         <v>13</v>
       </c>
       <c r="C50" s="103" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="D50" s="104"/>
       <c r="E50" s="102"/>
@@ -28244,7 +28252,7 @@
       <c r="A51" s="96"/>
       <c r="B51" s="106"/>
       <c r="C51" s="103" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="D51" s="104"/>
       <c r="E51" s="102"/>
@@ -28295,7 +28303,7 @@
       <c r="A52" s="96"/>
       <c r="B52" s="106"/>
       <c r="C52" s="103" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="D52" s="104"/>
       <c r="E52" s="102"/>
@@ -28345,7 +28353,7 @@
       <c r="A53" s="96"/>
       <c r="B53" s="106"/>
       <c r="C53" s="103" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="D53" s="104"/>
       <c r="E53" s="102"/>
@@ -28398,7 +28406,7 @@
         <v>14</v>
       </c>
       <c r="C54" s="103" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="D54" s="104"/>
       <c r="E54" s="102"/>
@@ -28451,7 +28459,7 @@
       <c r="A55" s="96"/>
       <c r="B55" s="106"/>
       <c r="C55" s="103" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="D55" s="104"/>
       <c r="E55" s="102"/>
@@ -28503,7 +28511,7 @@
       <c r="A56" s="96"/>
       <c r="B56" s="106"/>
       <c r="C56" s="103" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="D56" s="104"/>
       <c r="E56" s="102"/>
@@ -28554,7 +28562,7 @@
       <c r="A57" s="96"/>
       <c r="B57" s="106"/>
       <c r="C57" s="103" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="D57" s="104"/>
       <c r="E57" s="102"/>
@@ -28608,7 +28616,7 @@
         <v>15</v>
       </c>
       <c r="C58" s="103" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="D58" s="104"/>
       <c r="E58" s="102"/>
@@ -28662,7 +28670,7 @@
       <c r="A59" s="96"/>
       <c r="B59" s="126"/>
       <c r="C59" s="103" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="D59" s="104"/>
       <c r="E59" s="102"/>
@@ -28714,7 +28722,7 @@
       <c r="A60" s="96"/>
       <c r="B60" s="126"/>
       <c r="C60" s="103" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="D60" s="104"/>
       <c r="E60" s="102"/>
@@ -28766,7 +28774,7 @@
       <c r="A61" s="96"/>
       <c r="B61" s="126"/>
       <c r="C61" s="127" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="D61" s="128"/>
       <c r="E61" s="129"/>
@@ -28816,13 +28824,13 @@
     </row>
     <row r="62" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="96" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="B62" s="131" t="n">
         <v>16</v>
       </c>
       <c r="C62" s="103" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="D62" s="104"/>
       <c r="E62" s="102"/>
@@ -28841,7 +28849,7 @@
       <c r="R62" s="102"/>
       <c r="S62" s="102"/>
       <c r="T62" s="102" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="U62" s="102" t="n">
         <v>0</v>
@@ -28873,7 +28881,7 @@
       <c r="A63" s="96"/>
       <c r="B63" s="131"/>
       <c r="C63" s="103" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="D63" s="104"/>
       <c r="E63" s="102"/>
@@ -28892,7 +28900,7 @@
       <c r="R63" s="102"/>
       <c r="S63" s="102"/>
       <c r="T63" s="102" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="U63" s="102" t="n">
         <v>0</v>
@@ -28924,7 +28932,7 @@
       <c r="A64" s="96"/>
       <c r="B64" s="131"/>
       <c r="C64" s="103" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="D64" s="104"/>
       <c r="E64" s="102"/>
@@ -28943,7 +28951,7 @@
       <c r="R64" s="102"/>
       <c r="S64" s="102"/>
       <c r="T64" s="102" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="U64" s="102" t="n">
         <v>0</v>
@@ -28975,7 +28983,7 @@
       <c r="A65" s="96"/>
       <c r="B65" s="131"/>
       <c r="C65" s="103" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="D65" s="104"/>
       <c r="E65" s="102"/>
@@ -28994,7 +29002,7 @@
       <c r="R65" s="102"/>
       <c r="S65" s="102"/>
       <c r="T65" s="102" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="U65" s="102" t="n">
         <v>0</v>
@@ -29028,7 +29036,7 @@
         <v>17</v>
       </c>
       <c r="C66" s="103" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="D66" s="104"/>
       <c r="E66" s="102"/>
@@ -29047,7 +29055,7 @@
       <c r="R66" s="102"/>
       <c r="S66" s="102"/>
       <c r="T66" s="102" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="U66" s="102" t="n">
         <v>0</v>
@@ -29079,7 +29087,7 @@
       <c r="A67" s="96"/>
       <c r="B67" s="106"/>
       <c r="C67" s="103" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="D67" s="104"/>
       <c r="E67" s="102"/>
@@ -29098,7 +29106,7 @@
       <c r="R67" s="102"/>
       <c r="S67" s="102"/>
       <c r="T67" s="102" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="U67" s="102" t="n">
         <v>0</v>
@@ -29130,7 +29138,7 @@
       <c r="A68" s="96"/>
       <c r="B68" s="106"/>
       <c r="C68" s="103" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="D68" s="104"/>
       <c r="E68" s="102"/>
@@ -29149,7 +29157,7 @@
       <c r="R68" s="102"/>
       <c r="S68" s="102"/>
       <c r="T68" s="102" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="U68" s="102" t="n">
         <v>0</v>
@@ -29181,7 +29189,7 @@
       <c r="A69" s="96"/>
       <c r="B69" s="106"/>
       <c r="C69" s="103" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="D69" s="104"/>
       <c r="E69" s="102"/>
@@ -29200,7 +29208,7 @@
       <c r="R69" s="102"/>
       <c r="S69" s="102"/>
       <c r="T69" s="102" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="U69" s="102" t="n">
         <v>0</v>
@@ -29234,7 +29242,7 @@
         <v>18</v>
       </c>
       <c r="C70" s="103" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="D70" s="104"/>
       <c r="E70" s="102"/>
@@ -29253,7 +29261,7 @@
       <c r="R70" s="102"/>
       <c r="S70" s="102"/>
       <c r="T70" s="102" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="U70" s="102" t="n">
         <v>0</v>
@@ -29285,7 +29293,7 @@
       <c r="A71" s="96"/>
       <c r="B71" s="106"/>
       <c r="C71" s="103" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="D71" s="104"/>
       <c r="E71" s="102"/>
@@ -29304,7 +29312,7 @@
       <c r="R71" s="102"/>
       <c r="S71" s="102"/>
       <c r="T71" s="102" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="U71" s="102" t="n">
         <v>0</v>
@@ -29336,7 +29344,7 @@
       <c r="A72" s="96"/>
       <c r="B72" s="106"/>
       <c r="C72" s="103" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="D72" s="104"/>
       <c r="E72" s="102"/>
@@ -29355,7 +29363,7 @@
       <c r="R72" s="102"/>
       <c r="S72" s="102"/>
       <c r="T72" s="102" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="U72" s="102" t="n">
         <v>0</v>
@@ -29387,7 +29395,7 @@
       <c r="A73" s="96"/>
       <c r="B73" s="106"/>
       <c r="C73" s="103" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="D73" s="104"/>
       <c r="E73" s="102"/>
@@ -29406,7 +29414,7 @@
       <c r="R73" s="102"/>
       <c r="S73" s="102"/>
       <c r="T73" s="102" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="U73" s="102" t="n">
         <v>0</v>
@@ -29440,7 +29448,7 @@
         <v>19</v>
       </c>
       <c r="C74" s="103" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="D74" s="104"/>
       <c r="E74" s="102"/>
@@ -29459,7 +29467,7 @@
       <c r="R74" s="102"/>
       <c r="S74" s="102"/>
       <c r="T74" s="102" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="U74" s="102" t="n">
         <v>0</v>
@@ -29491,7 +29499,7 @@
       <c r="A75" s="96"/>
       <c r="B75" s="126"/>
       <c r="C75" s="103" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="D75" s="104"/>
       <c r="E75" s="102"/>
@@ -29510,7 +29518,7 @@
       <c r="R75" s="102"/>
       <c r="S75" s="102"/>
       <c r="T75" s="102" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="U75" s="102" t="n">
         <v>0</v>
@@ -29542,7 +29550,7 @@
       <c r="A76" s="96"/>
       <c r="B76" s="126"/>
       <c r="C76" s="103" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="D76" s="104"/>
       <c r="E76" s="102"/>
@@ -29561,7 +29569,7 @@
       <c r="R76" s="102"/>
       <c r="S76" s="102"/>
       <c r="T76" s="102" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="U76" s="102" t="n">
         <v>0</v>
@@ -29593,7 +29601,7 @@
       <c r="A77" s="96"/>
       <c r="B77" s="126"/>
       <c r="C77" s="127" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="D77" s="128"/>
       <c r="E77" s="129"/>
@@ -29612,7 +29620,7 @@
       <c r="R77" s="129"/>
       <c r="S77" s="129"/>
       <c r="T77" s="129" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="U77" s="129" t="n">
         <v>0</v>
@@ -29779,7 +29787,7 @@
       <c r="A80" s="102"/>
       <c r="B80" s="102"/>
       <c r="C80" s="136" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="D80" s="136"/>
       <c r="E80" s="101" t="n">
@@ -29805,7 +29813,7 @@
       <c r="W80" s="102"/>
       <c r="X80" s="102"/>
       <c r="Y80" s="137" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="Z80" s="102"/>
       <c r="AA80" s="102"/>
@@ -29821,7 +29829,7 @@
       <c r="A81" s="102"/>
       <c r="B81" s="102"/>
       <c r="C81" s="138" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="D81" s="138"/>
       <c r="E81" s="105" t="n">
@@ -29861,7 +29869,7 @@
       <c r="A82" s="102"/>
       <c r="B82" s="102"/>
       <c r="C82" s="138" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="D82" s="138"/>
       <c r="E82" s="105" t="n">
@@ -29901,7 +29909,7 @@
       <c r="A83" s="102"/>
       <c r="B83" s="102"/>
       <c r="C83" s="138" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="D83" s="138"/>
       <c r="E83" s="105" t="n">
@@ -29941,7 +29949,7 @@
       <c r="A84" s="102"/>
       <c r="B84" s="102"/>
       <c r="C84" s="138" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="D84" s="138"/>
       <c r="E84" s="105" t="n">
@@ -29981,7 +29989,7 @@
       <c r="A85" s="102"/>
       <c r="B85" s="102"/>
       <c r="C85" s="139" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="D85" s="139"/>
       <c r="E85" s="130" t="n">
@@ -30110,98 +30118,98 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="42" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="B4" s="140" t="n">
         <v>43739</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="B5" s="140" t="n">
         <v>44621</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="B6" s="141" t="n">
         <f aca="false">B5-B4</f>
         <v>882</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="B7" s="142" t="n">
         <f aca="false">B6/365</f>
         <v>2.41643835616438</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="B8" s="143" t="n">
         <v>7.5</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="42" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="C10" s="144" t="n">
         <f aca="false">260*B8*0.2*B7</f>
         <v>942.41095890411</v>
       </c>
       <c r="F10" s="145" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F11" s="145" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="42" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="C12" s="146" t="e">
         <f aca="false">'otjt log'!#ref!</f>
         <v>#VALUE!</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="42" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="C14" s="147" t="e">
         <f aca="false">C12-C10</f>
@@ -30210,7 +30218,7 @@
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="148" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
     </row>
   </sheetData>
@@ -30268,7 +30276,7 @@
     <row r="2" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2"/>
       <c r="B2" s="149" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="C2" s="150"/>
       <c r="D2" s="150"/>
@@ -30291,7 +30299,7 @@
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2"/>
       <c r="B3" s="152" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="C3" s="153"/>
       <c r="D3" s="153"/>
@@ -30314,7 +30322,7 @@
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2"/>
       <c r="B4" s="154" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="C4" s="153"/>
       <c r="D4" s="153"/>
@@ -30337,7 +30345,7 @@
     <row r="5" customFormat="false" ht="39" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="2"/>
       <c r="B5" s="155" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="C5" s="155"/>
       <c r="D5" s="155"/>
@@ -30360,7 +30368,7 @@
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2"/>
       <c r="B6" s="156" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="C6" s="156"/>
       <c r="D6" s="156"/>
@@ -30431,7 +30439,7 @@
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B10" s="162" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>